<commit_message>
Better Character Tooltips - Minor usability changes
 --- Removed dark red & blue colour from wealth & artifacts (unreadable in tooltips)
 --- Altered the wealth intervals (because many characters have 100 +/- 2; and because now have fewer easily-distinguishable colours)
</commit_message>
<xml_diff>
--- a/better_character_tooltips/generators/Custom Loc Generator.xlsx
+++ b/better_character_tooltips/generators/Custom Loc Generator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Health" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t xml:space="preserve">Base text:</t>
   </si>
@@ -170,16 +170,13 @@
     <t xml:space="preserve">AAA</t>
   </si>
   <si>
-    <t xml:space="preserve">Q</t>
+    <t xml:space="preserve">§!</t>
   </si>
   <si>
     <t xml:space="preserve">BBB</t>
   </si>
   <si>
-    <t xml:space="preserve">§YQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">§!</t>
+    <t xml:space="preserve">Q</t>
   </si>
   <si>
     <t xml:space="preserve">Replace text 3:</t>
@@ -188,7 +185,7 @@
     <t xml:space="preserve">CCC</t>
   </si>
   <si>
-    <t xml:space="preserve">§GQ</t>
+    <t xml:space="preserve">§YQ</t>
   </si>
   <si>
     <t xml:space="preserve">Replace text 4:</t>
@@ -197,7 +194,7 @@
     <t xml:space="preserve">DDD</t>
   </si>
   <si>
-    <t xml:space="preserve">§BQ</t>
+    <t xml:space="preserve">§GQ</t>
   </si>
   <si>
     <t xml:space="preserve">§PQ</t>
@@ -476,7 +473,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5211,7 +5208,7 @@
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
@@ -5268,8 +5265,7 @@
       </c>
       <c r="B5" s="14" t="str">
         <f aca="false">_xlfn.TEXTJOIN("",0,$C$8:$C$19)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Haughty
     use_first_valid = yes
     text = {
@@ -5437,8 +5433,7 @@
       </c>
       <c r="C8" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A8),$B$3,B8)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Haughty
     use_first_valid = yes
     text = {
@@ -5462,8 +5457,7 @@
       </c>
       <c r="C9" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A9),$B$3,B9)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Affectionate
     use_first_valid = yes
     text = {
@@ -5487,8 +5481,7 @@
       </c>
       <c r="C10" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A10),$B$3,B10)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Timid
     use_first_valid = yes
     text = {
@@ -5512,8 +5505,7 @@
       </c>
       <c r="C11" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A11),$B$3,B11)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Rowdy
     use_first_valid = yes
     text = {
@@ -5537,8 +5529,7 @@
       </c>
       <c r="C12" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A12),$B$3,B12)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Willful
     use_first_valid = yes
     text = {
@@ -5562,8 +5553,7 @@
       </c>
       <c r="C13" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A13),$B$3,B13)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Brooding
     use_first_valid = yes
     text = {
@@ -5587,8 +5577,7 @@
       </c>
       <c r="C14" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A14),$B$3,B14)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Indolent
     use_first_valid = yes
     text = {
@@ -5612,8 +5601,7 @@
       </c>
       <c r="C15" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A15),$B$3,B15)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Playful
     use_first_valid = yes
     text = {
@@ -5637,8 +5625,7 @@
       </c>
       <c r="C16" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A16),$B$3,B16)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Conscientious
     use_first_valid = yes
     text = {
@@ -5662,8 +5649,7 @@
       </c>
       <c r="C17" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A17),$B$3,B17)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Fussy
     use_first_valid = yes
     text = {
@@ -5687,8 +5673,7 @@
       </c>
       <c r="C18" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A18),$B$3,B18)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Curious
     use_first_valid = yes
     text = {
@@ -5712,8 +5697,7 @@
       </c>
       <c r="C19" s="9" t="str">
         <f aca="false">$B$4&amp;SUBSTITUTE(SUBSTITUTE($B$1,$B$2,A19),$B$3,B19)</f>
-        <v>
-defined_text = {
+        <v>defined_text = {
     name = BCT_Childhood_Idolizer
     use_first_valid = yes
     text = {
@@ -5745,10 +5729,10 @@
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5785,10 +5769,13 @@
       <c r="E2" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="17" t="str">
+        <f aca="false">"§gQ"</f>
+        <v>§gQ</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -5803,42 +5790,40 @@
       <c r="F3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>44</v>
-      </c>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E4" s="17" t="n">
         <v>3</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E5" s="17" t="n">
         <v>4</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5854,10 +5839,10 @@
         <v>5</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5866,26 +5851,27 @@
       </c>
       <c r="B7" s="14" t="str">
         <f aca="false">_xlfn.TEXTJOIN("",0,$G$12:$G$56)</f>
-        <v>BCT_Artifacts_Q1_1;1 x Q1;;;;;;;;;;;;;x
-BCT_Artifacts_Q1_2;2 x Q1;;;;;;;;;;;;;x
-BCT_Artifacts_Q1_3;3 x Q1;;;;;;;;;;;;;x
-BCT_Artifacts_Q1_4;4 x Q1;;;;;;;;;;;;;x
-BCT_Artifacts_Q1_5;5+ x Q1;;;;;;;;;;;;;x
-BCT_Artifacts_Q2_1;1 x §YQ2§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q2_2;2 x §YQ2§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q2_3;3 x §YQ2§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q2_4;4 x §YQ2§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q2_5;5+ x §YQ2§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_1;1 x §GQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_2;2 x §GQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_3;3 x §GQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_4;4 x §GQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_5;5+ x §GQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q4_1;1 x §BQ4§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q4_2;2 x §BQ4§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q4_3;3 x §BQ4§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q4_4;4 x §BQ4§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q4_5;5+ x §BQ4§!;;;;;;;;;;;;;x
+        <v>
+BCT_Artifacts_Q1_1;1 x §gQ1§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q1_2;2 x §gQ1§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q1_3;3 x §gQ1§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q1_4;4 x §gQ1§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q1_5;5+ x §gQ1§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q2_1;1 x Q2;;;;;;;;;;;;;x
+BCT_Artifacts_Q2_2;2 x Q2;;;;;;;;;;;;;x
+BCT_Artifacts_Q2_3;3 x Q2;;;;;;;;;;;;;x
+BCT_Artifacts_Q2_4;4 x Q2;;;;;;;;;;;;;x
+BCT_Artifacts_Q2_5;5+ x Q2;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_1;1 x §YQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_2;2 x §YQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_3;3 x §YQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_4;4 x §YQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_5;5+ x §YQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q4_1;1 x §GQ4§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q4_2;2 x §GQ4§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q4_3;3 x §GQ4§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q4_4;4 x §GQ4§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q4_5;5+ x §GQ4§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q5_1;1 x §PQ5§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q5_2;2 x §PQ5§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q5_3;3 x §PQ5§!;;;;;;;;;;;;;x
@@ -5916,10 +5902,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5927,10 +5913,10 @@
         <v>7</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5938,10 +5924,10 @@
         <v>8</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5949,30 +5935,30 @@
         <v>9</v>
       </c>
       <c r="F10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>13</v>
@@ -5996,7 +5982,7 @@
       </c>
       <c r="E12" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A12,$E$2:$E$10,1))&amp;C12&amp;INDEX($G$2:$G$10,MATCH(A12,$E$2:$E$10,1))</f>
-        <v>Q1</v>
+        <v>§gQ1§!</v>
       </c>
       <c r="F12" s="20" t="str">
         <f aca="false">D12&amp;IF(B12=$E$6,"+","")</f>
@@ -6004,7 +5990,8 @@
       </c>
       <c r="G12" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C12),$B$3,D12),$B$4,E12),$B$5,F12)</f>
-        <v>BCT_Artifacts_Q1_1;1 x Q1;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q1_1;1 x §gQ1§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6026,7 +6013,7 @@
       </c>
       <c r="E13" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A13,$E$2:$E$10,1))&amp;C13&amp;INDEX($G$2:$G$10,MATCH(A13,$E$2:$E$10,1))</f>
-        <v>Q1</v>
+        <v>§gQ1§!</v>
       </c>
       <c r="F13" s="20" t="str">
         <f aca="false">D13&amp;IF(B13=$E$6,"+","")</f>
@@ -6034,7 +6021,8 @@
       </c>
       <c r="G13" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C13),$B$3,D13),$B$4,E13),$B$5,F13)</f>
-        <v>BCT_Artifacts_Q1_2;2 x Q1;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q1_2;2 x §gQ1§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6056,7 +6044,7 @@
       </c>
       <c r="E14" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A14,$E$2:$E$10,1))&amp;C14&amp;INDEX($G$2:$G$10,MATCH(A14,$E$2:$E$10,1))</f>
-        <v>Q1</v>
+        <v>§gQ1§!</v>
       </c>
       <c r="F14" s="20" t="str">
         <f aca="false">D14&amp;IF(B14=$E$6,"+","")</f>
@@ -6064,7 +6052,8 @@
       </c>
       <c r="G14" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C14),$B$3,D14),$B$4,E14),$B$5,F14)</f>
-        <v>BCT_Artifacts_Q1_3;3 x Q1;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q1_3;3 x §gQ1§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6086,7 +6075,7 @@
       </c>
       <c r="E15" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A15,$E$2:$E$10,1))&amp;C15&amp;INDEX($G$2:$G$10,MATCH(A15,$E$2:$E$10,1))</f>
-        <v>Q1</v>
+        <v>§gQ1§!</v>
       </c>
       <c r="F15" s="20" t="str">
         <f aca="false">D15&amp;IF(B15=$E$6,"+","")</f>
@@ -6094,7 +6083,8 @@
       </c>
       <c r="G15" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C15),$B$3,D15),$B$4,E15),$B$5,F15)</f>
-        <v>BCT_Artifacts_Q1_4;4 x Q1;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q1_4;4 x §gQ1§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6116,7 +6106,7 @@
       </c>
       <c r="E16" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A16,$E$2:$E$10,1))&amp;C16&amp;INDEX($G$2:$G$10,MATCH(A16,$E$2:$E$10,1))</f>
-        <v>Q1</v>
+        <v>§gQ1§!</v>
       </c>
       <c r="F16" s="20" t="str">
         <f aca="false">D16&amp;IF(B16=$E$6,"+","")</f>
@@ -6124,7 +6114,8 @@
       </c>
       <c r="G16" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C16),$B$3,D16),$B$4,E16),$B$5,F16)</f>
-        <v>BCT_Artifacts_Q1_5;5+ x Q1;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q1_5;5+ x §gQ1§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6146,7 +6137,7 @@
       </c>
       <c r="E17" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A17,$E$2:$E$10,1))&amp;C17&amp;INDEX($G$2:$G$10,MATCH(A17,$E$2:$E$10,1))</f>
-        <v>§YQ2§!</v>
+        <v>Q2</v>
       </c>
       <c r="F17" s="20" t="str">
         <f aca="false">D17&amp;IF(B17=$E$6,"+","")</f>
@@ -6154,7 +6145,8 @@
       </c>
       <c r="G17" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C17),$B$3,D17),$B$4,E17),$B$5,F17)</f>
-        <v>BCT_Artifacts_Q2_1;1 x §YQ2§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q2_1;1 x Q2;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6176,7 +6168,7 @@
       </c>
       <c r="E18" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A18,$E$2:$E$10,1))&amp;C18&amp;INDEX($G$2:$G$10,MATCH(A18,$E$2:$E$10,1))</f>
-        <v>§YQ2§!</v>
+        <v>Q2</v>
       </c>
       <c r="F18" s="20" t="str">
         <f aca="false">D18&amp;IF(B18=$E$6,"+","")</f>
@@ -6184,7 +6176,8 @@
       </c>
       <c r="G18" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C18),$B$3,D18),$B$4,E18),$B$5,F18)</f>
-        <v>BCT_Artifacts_Q2_2;2 x §YQ2§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q2_2;2 x Q2;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6206,7 +6199,7 @@
       </c>
       <c r="E19" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A19,$E$2:$E$10,1))&amp;C19&amp;INDEX($G$2:$G$10,MATCH(A19,$E$2:$E$10,1))</f>
-        <v>§YQ2§!</v>
+        <v>Q2</v>
       </c>
       <c r="F19" s="20" t="str">
         <f aca="false">D19&amp;IF(B19=$E$6,"+","")</f>
@@ -6214,7 +6207,8 @@
       </c>
       <c r="G19" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C19),$B$3,D19),$B$4,E19),$B$5,F19)</f>
-        <v>BCT_Artifacts_Q2_3;3 x §YQ2§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q2_3;3 x Q2;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6236,7 +6230,7 @@
       </c>
       <c r="E20" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A20,$E$2:$E$10,1))&amp;C20&amp;INDEX($G$2:$G$10,MATCH(A20,$E$2:$E$10,1))</f>
-        <v>§YQ2§!</v>
+        <v>Q2</v>
       </c>
       <c r="F20" s="20" t="str">
         <f aca="false">D20&amp;IF(B20=$E$6,"+","")</f>
@@ -6244,7 +6238,8 @@
       </c>
       <c r="G20" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C20),$B$3,D20),$B$4,E20),$B$5,F20)</f>
-        <v>BCT_Artifacts_Q2_4;4 x §YQ2§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q2_4;4 x Q2;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6266,7 +6261,7 @@
       </c>
       <c r="E21" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A21,$E$2:$E$10,1))&amp;C21&amp;INDEX($G$2:$G$10,MATCH(A21,$E$2:$E$10,1))</f>
-        <v>§YQ2§!</v>
+        <v>Q2</v>
       </c>
       <c r="F21" s="20" t="str">
         <f aca="false">D21&amp;IF(B21=$E$6,"+","")</f>
@@ -6274,7 +6269,8 @@
       </c>
       <c r="G21" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C21),$B$3,D21),$B$4,E21),$B$5,F21)</f>
-        <v>BCT_Artifacts_Q2_5;5+ x §YQ2§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q2_5;5+ x Q2;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6296,7 +6292,7 @@
       </c>
       <c r="E22" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A22,$E$2:$E$10,1))&amp;C22&amp;INDEX($G$2:$G$10,MATCH(A22,$E$2:$E$10,1))</f>
-        <v>§GQ3§!</v>
+        <v>§YQ3§!</v>
       </c>
       <c r="F22" s="20" t="str">
         <f aca="false">D22&amp;IF(B22=$E$6,"+","")</f>
@@ -6304,7 +6300,8 @@
       </c>
       <c r="G22" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C22),$B$3,D22),$B$4,E22),$B$5,F22)</f>
-        <v>BCT_Artifacts_Q3_1;1 x §GQ3§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q3_1;1 x §YQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6326,7 +6323,7 @@
       </c>
       <c r="E23" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A23,$E$2:$E$10,1))&amp;C23&amp;INDEX($G$2:$G$10,MATCH(A23,$E$2:$E$10,1))</f>
-        <v>§GQ3§!</v>
+        <v>§YQ3§!</v>
       </c>
       <c r="F23" s="20" t="str">
         <f aca="false">D23&amp;IF(B23=$E$6,"+","")</f>
@@ -6334,7 +6331,8 @@
       </c>
       <c r="G23" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C23),$B$3,D23),$B$4,E23),$B$5,F23)</f>
-        <v>BCT_Artifacts_Q3_2;2 x §GQ3§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q3_2;2 x §YQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6356,7 +6354,7 @@
       </c>
       <c r="E24" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A24,$E$2:$E$10,1))&amp;C24&amp;INDEX($G$2:$G$10,MATCH(A24,$E$2:$E$10,1))</f>
-        <v>§GQ3§!</v>
+        <v>§YQ3§!</v>
       </c>
       <c r="F24" s="20" t="str">
         <f aca="false">D24&amp;IF(B24=$E$6,"+","")</f>
@@ -6364,7 +6362,8 @@
       </c>
       <c r="G24" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C24),$B$3,D24),$B$4,E24),$B$5,F24)</f>
-        <v>BCT_Artifacts_Q3_3;3 x §GQ3§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q3_3;3 x §YQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6386,7 +6385,7 @@
       </c>
       <c r="E25" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A25,$E$2:$E$10,1))&amp;C25&amp;INDEX($G$2:$G$10,MATCH(A25,$E$2:$E$10,1))</f>
-        <v>§GQ3§!</v>
+        <v>§YQ3§!</v>
       </c>
       <c r="F25" s="20" t="str">
         <f aca="false">D25&amp;IF(B25=$E$6,"+","")</f>
@@ -6394,7 +6393,8 @@
       </c>
       <c r="G25" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C25),$B$3,D25),$B$4,E25),$B$5,F25)</f>
-        <v>BCT_Artifacts_Q3_4;4 x §GQ3§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q3_4;4 x §YQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="E26" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A26,$E$2:$E$10,1))&amp;C26&amp;INDEX($G$2:$G$10,MATCH(A26,$E$2:$E$10,1))</f>
-        <v>§GQ3§!</v>
+        <v>§YQ3§!</v>
       </c>
       <c r="F26" s="20" t="str">
         <f aca="false">D26&amp;IF(B26=$E$6,"+","")</f>
@@ -6424,7 +6424,8 @@
       </c>
       <c r="G26" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C26),$B$3,D26),$B$4,E26),$B$5,F26)</f>
-        <v>BCT_Artifacts_Q3_5;5+ x §GQ3§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q3_5;5+ x §YQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6446,7 +6447,7 @@
       </c>
       <c r="E27" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A27,$E$2:$E$10,1))&amp;C27&amp;INDEX($G$2:$G$10,MATCH(A27,$E$2:$E$10,1))</f>
-        <v>§BQ4§!</v>
+        <v>§GQ4§!</v>
       </c>
       <c r="F27" s="20" t="str">
         <f aca="false">D27&amp;IF(B27=$E$6,"+","")</f>
@@ -6454,7 +6455,8 @@
       </c>
       <c r="G27" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C27),$B$3,D27),$B$4,E27),$B$5,F27)</f>
-        <v>BCT_Artifacts_Q4_1;1 x §BQ4§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q4_1;1 x §GQ4§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6476,7 +6478,7 @@
       </c>
       <c r="E28" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A28,$E$2:$E$10,1))&amp;C28&amp;INDEX($G$2:$G$10,MATCH(A28,$E$2:$E$10,1))</f>
-        <v>§BQ4§!</v>
+        <v>§GQ4§!</v>
       </c>
       <c r="F28" s="20" t="str">
         <f aca="false">D28&amp;IF(B28=$E$6,"+","")</f>
@@ -6484,7 +6486,8 @@
       </c>
       <c r="G28" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C28),$B$3,D28),$B$4,E28),$B$5,F28)</f>
-        <v>BCT_Artifacts_Q4_2;2 x §BQ4§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q4_2;2 x §GQ4§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6506,7 +6509,7 @@
       </c>
       <c r="E29" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A29,$E$2:$E$10,1))&amp;C29&amp;INDEX($G$2:$G$10,MATCH(A29,$E$2:$E$10,1))</f>
-        <v>§BQ4§!</v>
+        <v>§GQ4§!</v>
       </c>
       <c r="F29" s="20" t="str">
         <f aca="false">D29&amp;IF(B29=$E$6,"+","")</f>
@@ -6514,7 +6517,8 @@
       </c>
       <c r="G29" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C29),$B$3,D29),$B$4,E29),$B$5,F29)</f>
-        <v>BCT_Artifacts_Q4_3;3 x §BQ4§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q4_3;3 x §GQ4§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6536,7 +6540,7 @@
       </c>
       <c r="E30" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A30,$E$2:$E$10,1))&amp;C30&amp;INDEX($G$2:$G$10,MATCH(A30,$E$2:$E$10,1))</f>
-        <v>§BQ4§!</v>
+        <v>§GQ4§!</v>
       </c>
       <c r="F30" s="20" t="str">
         <f aca="false">D30&amp;IF(B30=$E$6,"+","")</f>
@@ -6544,7 +6548,8 @@
       </c>
       <c r="G30" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C30),$B$3,D30),$B$4,E30),$B$5,F30)</f>
-        <v>BCT_Artifacts_Q4_4;4 x §BQ4§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q4_4;4 x §GQ4§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6566,7 +6571,7 @@
       </c>
       <c r="E31" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A31,$E$2:$E$10,1))&amp;C31&amp;INDEX($G$2:$G$10,MATCH(A31,$E$2:$E$10,1))</f>
-        <v>§BQ4§!</v>
+        <v>§GQ4§!</v>
       </c>
       <c r="F31" s="20" t="str">
         <f aca="false">D31&amp;IF(B31=$E$6,"+","")</f>
@@ -6574,7 +6579,8 @@
       </c>
       <c r="G31" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C31),$B$3,D31),$B$4,E31),$B$5,F31)</f>
-        <v>BCT_Artifacts_Q4_5;5+ x §BQ4§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q4_5;5+ x §GQ4§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6604,7 +6610,8 @@
       </c>
       <c r="G32" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C32),$B$3,D32),$B$4,E32),$B$5,F32)</f>
-        <v>BCT_Artifacts_Q5_1;1 x §PQ5§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q5_1;1 x §PQ5§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6634,7 +6641,8 @@
       </c>
       <c r="G33" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C33),$B$3,D33),$B$4,E33),$B$5,F33)</f>
-        <v>BCT_Artifacts_Q5_2;2 x §PQ5§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q5_2;2 x §PQ5§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6664,7 +6672,8 @@
       </c>
       <c r="G34" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C34),$B$3,D34),$B$4,E34),$B$5,F34)</f>
-        <v>BCT_Artifacts_Q5_3;3 x §PQ5§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q5_3;3 x §PQ5§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6694,7 +6703,8 @@
       </c>
       <c r="G35" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C35),$B$3,D35),$B$4,E35),$B$5,F35)</f>
-        <v>BCT_Artifacts_Q5_4;4 x §PQ5§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q5_4;4 x §PQ5§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6724,7 +6734,8 @@
       </c>
       <c r="G36" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C36),$B$3,D36),$B$4,E36),$B$5,F36)</f>
-        <v>BCT_Artifacts_Q5_5;5+ x §PQ5§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q5_5;5+ x §PQ5§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6754,7 +6765,8 @@
       </c>
       <c r="G37" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C37),$B$3,D37),$B$4,E37),$B$5,F37)</f>
-        <v>BCT_Artifacts_Q6_1;1 x §MQ6§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q6_1;1 x §MQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6784,7 +6796,8 @@
       </c>
       <c r="G38" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C38),$B$3,D38),$B$4,E38),$B$5,F38)</f>
-        <v>BCT_Artifacts_Q6_2;2 x §MQ6§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q6_2;2 x §MQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6814,7 +6827,8 @@
       </c>
       <c r="G39" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C39),$B$3,D39),$B$4,E39),$B$5,F39)</f>
-        <v>BCT_Artifacts_Q6_3;3 x §MQ6§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q6_3;3 x §MQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6844,7 +6858,8 @@
       </c>
       <c r="G40" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C40),$B$3,D40),$B$4,E40),$B$5,F40)</f>
-        <v>BCT_Artifacts_Q6_4;4 x §MQ6§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q6_4;4 x §MQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6874,7 +6889,8 @@
       </c>
       <c r="G41" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C41),$B$3,D41),$B$4,E41),$B$5,F41)</f>
-        <v>BCT_Artifacts_Q6_5;5+ x §MQ6§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q6_5;5+ x §MQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6904,7 +6920,8 @@
       </c>
       <c r="G42" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C42),$B$3,D42),$B$4,E42),$B$5,F42)</f>
-        <v>BCT_Artifacts_Q7_1;1 x §MQ7§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q7_1;1 x §MQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6934,7 +6951,8 @@
       </c>
       <c r="G43" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C43),$B$3,D43),$B$4,E43),$B$5,F43)</f>
-        <v>BCT_Artifacts_Q7_2;2 x §MQ7§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q7_2;2 x §MQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6964,7 +6982,8 @@
       </c>
       <c r="G44" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C44),$B$3,D44),$B$4,E44),$B$5,F44)</f>
-        <v>BCT_Artifacts_Q7_3;3 x §MQ7§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q7_3;3 x §MQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6994,7 +7013,8 @@
       </c>
       <c r="G45" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C45),$B$3,D45),$B$4,E45),$B$5,F45)</f>
-        <v>BCT_Artifacts_Q7_4;4 x §MQ7§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q7_4;4 x §MQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7024,7 +7044,8 @@
       </c>
       <c r="G46" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C46),$B$3,D46),$B$4,E46),$B$5,F46)</f>
-        <v>BCT_Artifacts_Q7_5;5+ x §MQ7§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q7_5;5+ x §MQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7054,7 +7075,8 @@
       </c>
       <c r="G47" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C47),$B$3,D47),$B$4,E47),$B$5,F47)</f>
-        <v>BCT_Artifacts_Q8_1;1 x §lQ8§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q8_1;1 x §lQ8§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7084,7 +7106,8 @@
       </c>
       <c r="G48" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C48),$B$3,D48),$B$4,E48),$B$5,F48)</f>
-        <v>BCT_Artifacts_Q8_2;2 x §lQ8§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q8_2;2 x §lQ8§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7114,7 +7137,8 @@
       </c>
       <c r="G49" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C49),$B$3,D49),$B$4,E49),$B$5,F49)</f>
-        <v>BCT_Artifacts_Q8_3;3 x §lQ8§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q8_3;3 x §lQ8§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7144,7 +7168,8 @@
       </c>
       <c r="G50" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C50),$B$3,D50),$B$4,E50),$B$5,F50)</f>
-        <v>BCT_Artifacts_Q8_4;4 x §lQ8§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q8_4;4 x §lQ8§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7174,7 +7199,8 @@
       </c>
       <c r="G51" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C51),$B$3,D51),$B$4,E51),$B$5,F51)</f>
-        <v>BCT_Artifacts_Q8_5;5+ x §lQ8§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q8_5;5+ x §lQ8§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7204,7 +7230,8 @@
       </c>
       <c r="G52" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C52),$B$3,D52),$B$4,E52),$B$5,F52)</f>
-        <v>BCT_Artifacts_Q9_1;1 x §lQ9+§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q9_1;1 x §lQ9+§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7234,7 +7261,8 @@
       </c>
       <c r="G53" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C53),$B$3,D53),$B$4,E53),$B$5,F53)</f>
-        <v>BCT_Artifacts_Q9_2;2 x §lQ9+§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q9_2;2 x §lQ9+§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7264,7 +7292,8 @@
       </c>
       <c r="G54" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C54),$B$3,D54),$B$4,E54),$B$5,F54)</f>
-        <v>BCT_Artifacts_Q9_3;3 x §lQ9+§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q9_3;3 x §lQ9+§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7294,7 +7323,8 @@
       </c>
       <c r="G55" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C55),$B$3,D55),$B$4,E55),$B$5,F55)</f>
-        <v>BCT_Artifacts_Q9_4;4 x §lQ9+§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q9_4;4 x §lQ9+§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7324,7 +7354,8 @@
       </c>
       <c r="G56" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C56),$B$3,D56),$B$4,E56),$B$5,F56)</f>
-        <v>BCT_Artifacts_Q9_5;5+ x §lQ9+§!;;;;;;;;;;;;;x</v>
+        <v>
+BCT_Artifacts_Q9_5;5+ x §lQ9+§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better Character Tooltips - Use bright (instead of ordinary) yellow for medium-level wealth & artifacts
</commit_message>
<xml_diff>
--- a/better_character_tooltips/generators/Custom Loc Generator.xlsx
+++ b/better_character_tooltips/generators/Custom Loc Generator.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t xml:space="preserve">Base text:</t>
   </si>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">CCC</t>
   </si>
   <si>
-    <t xml:space="preserve">§YQ</t>
+    <t xml:space="preserve">§MQ</t>
   </si>
   <si>
     <t xml:space="preserve">Replace text 4:</t>
@@ -198,9 +198,6 @@
   </si>
   <si>
     <t xml:space="preserve">§PQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">§MQ</t>
   </si>
   <si>
     <t xml:space="preserve">§lQ</t>
@@ -5729,10 +5726,10 @@
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5862,11 +5859,11 @@
 BCT_Artifacts_Q2_3;3 x Q2;;;;;;;;;;;;;x
 BCT_Artifacts_Q2_4;4 x Q2;;;;;;;;;;;;;x
 BCT_Artifacts_Q2_5;5+ x Q2;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_1;1 x §YQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_2;2 x §YQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_3;3 x §YQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_4;4 x §YQ3§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q3_5;5+ x §YQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_1;1 x §MQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_2;2 x §MQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_3;3 x §MQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_4;4 x §MQ3§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q3_5;5+ x §MQ3§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q4_1;1 x §GQ4§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q4_2;2 x §GQ4§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q4_3;3 x §GQ4§!;;;;;;;;;;;;;x
@@ -5877,16 +5874,16 @@
 BCT_Artifacts_Q5_3;3 x §PQ5§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q5_4;4 x §PQ5§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q5_5;5+ x §PQ5§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q6_1;1 x §MQ6§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q6_2;2 x §MQ6§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q6_3;3 x §MQ6§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q6_4;4 x §MQ6§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q6_5;5+ x §MQ6§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q7_1;1 x §MQ7§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q7_2;2 x §MQ7§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q7_3;3 x §MQ7§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q7_4;4 x §MQ7§!;;;;;;;;;;;;;x
-BCT_Artifacts_Q7_5;5+ x §MQ7§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q6_1;1 x §lQ6§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q6_2;2 x §lQ6§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q6_3;3 x §lQ6§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q6_4;4 x §lQ6§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q6_5;5+ x §lQ6§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q7_1;1 x §lQ7§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q7_2;2 x §lQ7§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q7_3;3 x §lQ7§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q7_4;4 x §lQ7§!;;;;;;;;;;;;;x
+BCT_Artifacts_Q7_5;5+ x §lQ7§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q8_1;1 x §lQ8§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q8_2;2 x §lQ8§!;;;;;;;;;;;;;x
 BCT_Artifacts_Q8_3;3 x §lQ8§!;;;;;;;;;;;;;x
@@ -5924,7 +5921,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>41</v>
@@ -5935,30 +5932,30 @@
         <v>9</v>
       </c>
       <c r="F10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>13</v>
@@ -6292,7 +6289,7 @@
       </c>
       <c r="E22" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A22,$E$2:$E$10,1))&amp;C22&amp;INDEX($G$2:$G$10,MATCH(A22,$E$2:$E$10,1))</f>
-        <v>§YQ3§!</v>
+        <v>§MQ3§!</v>
       </c>
       <c r="F22" s="20" t="str">
         <f aca="false">D22&amp;IF(B22=$E$6,"+","")</f>
@@ -6301,7 +6298,7 @@
       <c r="G22" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C22),$B$3,D22),$B$4,E22),$B$5,F22)</f>
         <v>
-BCT_Artifacts_Q3_1;1 x §YQ3§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q3_1;1 x §MQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6323,7 +6320,7 @@
       </c>
       <c r="E23" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A23,$E$2:$E$10,1))&amp;C23&amp;INDEX($G$2:$G$10,MATCH(A23,$E$2:$E$10,1))</f>
-        <v>§YQ3§!</v>
+        <v>§MQ3§!</v>
       </c>
       <c r="F23" s="20" t="str">
         <f aca="false">D23&amp;IF(B23=$E$6,"+","")</f>
@@ -6332,7 +6329,7 @@
       <c r="G23" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C23),$B$3,D23),$B$4,E23),$B$5,F23)</f>
         <v>
-BCT_Artifacts_Q3_2;2 x §YQ3§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q3_2;2 x §MQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6354,7 +6351,7 @@
       </c>
       <c r="E24" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A24,$E$2:$E$10,1))&amp;C24&amp;INDEX($G$2:$G$10,MATCH(A24,$E$2:$E$10,1))</f>
-        <v>§YQ3§!</v>
+        <v>§MQ3§!</v>
       </c>
       <c r="F24" s="20" t="str">
         <f aca="false">D24&amp;IF(B24=$E$6,"+","")</f>
@@ -6363,7 +6360,7 @@
       <c r="G24" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C24),$B$3,D24),$B$4,E24),$B$5,F24)</f>
         <v>
-BCT_Artifacts_Q3_3;3 x §YQ3§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q3_3;3 x §MQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6385,7 +6382,7 @@
       </c>
       <c r="E25" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A25,$E$2:$E$10,1))&amp;C25&amp;INDEX($G$2:$G$10,MATCH(A25,$E$2:$E$10,1))</f>
-        <v>§YQ3§!</v>
+        <v>§MQ3§!</v>
       </c>
       <c r="F25" s="20" t="str">
         <f aca="false">D25&amp;IF(B25=$E$6,"+","")</f>
@@ -6394,7 +6391,7 @@
       <c r="G25" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C25),$B$3,D25),$B$4,E25),$B$5,F25)</f>
         <v>
-BCT_Artifacts_Q3_4;4 x §YQ3§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q3_4;4 x §MQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6416,7 +6413,7 @@
       </c>
       <c r="E26" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A26,$E$2:$E$10,1))&amp;C26&amp;INDEX($G$2:$G$10,MATCH(A26,$E$2:$E$10,1))</f>
-        <v>§YQ3§!</v>
+        <v>§MQ3§!</v>
       </c>
       <c r="F26" s="20" t="str">
         <f aca="false">D26&amp;IF(B26=$E$6,"+","")</f>
@@ -6425,7 +6422,7 @@
       <c r="G26" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C26),$B$3,D26),$B$4,E26),$B$5,F26)</f>
         <v>
-BCT_Artifacts_Q3_5;5+ x §YQ3§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q3_5;5+ x §MQ3§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6757,7 +6754,7 @@
       </c>
       <c r="E37" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A37,$E$2:$E$10,1))&amp;C37&amp;INDEX($G$2:$G$10,MATCH(A37,$E$2:$E$10,1))</f>
-        <v>§MQ6§!</v>
+        <v>§lQ6§!</v>
       </c>
       <c r="F37" s="20" t="str">
         <f aca="false">D37&amp;IF(B37=$E$6,"+","")</f>
@@ -6766,7 +6763,7 @@
       <c r="G37" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C37),$B$3,D37),$B$4,E37),$B$5,F37)</f>
         <v>
-BCT_Artifacts_Q6_1;1 x §MQ6§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q6_1;1 x §lQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6788,7 +6785,7 @@
       </c>
       <c r="E38" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A38,$E$2:$E$10,1))&amp;C38&amp;INDEX($G$2:$G$10,MATCH(A38,$E$2:$E$10,1))</f>
-        <v>§MQ6§!</v>
+        <v>§lQ6§!</v>
       </c>
       <c r="F38" s="20" t="str">
         <f aca="false">D38&amp;IF(B38=$E$6,"+","")</f>
@@ -6797,7 +6794,7 @@
       <c r="G38" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C38),$B$3,D38),$B$4,E38),$B$5,F38)</f>
         <v>
-BCT_Artifacts_Q6_2;2 x §MQ6§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q6_2;2 x §lQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6819,7 +6816,7 @@
       </c>
       <c r="E39" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A39,$E$2:$E$10,1))&amp;C39&amp;INDEX($G$2:$G$10,MATCH(A39,$E$2:$E$10,1))</f>
-        <v>§MQ6§!</v>
+        <v>§lQ6§!</v>
       </c>
       <c r="F39" s="20" t="str">
         <f aca="false">D39&amp;IF(B39=$E$6,"+","")</f>
@@ -6828,7 +6825,7 @@
       <c r="G39" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C39),$B$3,D39),$B$4,E39),$B$5,F39)</f>
         <v>
-BCT_Artifacts_Q6_3;3 x §MQ6§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q6_3;3 x §lQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6850,7 +6847,7 @@
       </c>
       <c r="E40" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A40,$E$2:$E$10,1))&amp;C40&amp;INDEX($G$2:$G$10,MATCH(A40,$E$2:$E$10,1))</f>
-        <v>§MQ6§!</v>
+        <v>§lQ6§!</v>
       </c>
       <c r="F40" s="20" t="str">
         <f aca="false">D40&amp;IF(B40=$E$6,"+","")</f>
@@ -6859,7 +6856,7 @@
       <c r="G40" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C40),$B$3,D40),$B$4,E40),$B$5,F40)</f>
         <v>
-BCT_Artifacts_Q6_4;4 x §MQ6§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q6_4;4 x §lQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6881,7 +6878,7 @@
       </c>
       <c r="E41" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A41,$E$2:$E$10,1))&amp;C41&amp;INDEX($G$2:$G$10,MATCH(A41,$E$2:$E$10,1))</f>
-        <v>§MQ6§!</v>
+        <v>§lQ6§!</v>
       </c>
       <c r="F41" s="20" t="str">
         <f aca="false">D41&amp;IF(B41=$E$6,"+","")</f>
@@ -6890,7 +6887,7 @@
       <c r="G41" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C41),$B$3,D41),$B$4,E41),$B$5,F41)</f>
         <v>
-BCT_Artifacts_Q6_5;5+ x §MQ6§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q6_5;5+ x §lQ6§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6912,7 +6909,7 @@
       </c>
       <c r="E42" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A42,$E$2:$E$10,1))&amp;C42&amp;INDEX($G$2:$G$10,MATCH(A42,$E$2:$E$10,1))</f>
-        <v>§MQ7§!</v>
+        <v>§lQ7§!</v>
       </c>
       <c r="F42" s="20" t="str">
         <f aca="false">D42&amp;IF(B42=$E$6,"+","")</f>
@@ -6921,7 +6918,7 @@
       <c r="G42" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C42),$B$3,D42),$B$4,E42),$B$5,F42)</f>
         <v>
-BCT_Artifacts_Q7_1;1 x §MQ7§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q7_1;1 x §lQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6943,7 +6940,7 @@
       </c>
       <c r="E43" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A43,$E$2:$E$10,1))&amp;C43&amp;INDEX($G$2:$G$10,MATCH(A43,$E$2:$E$10,1))</f>
-        <v>§MQ7§!</v>
+        <v>§lQ7§!</v>
       </c>
       <c r="F43" s="20" t="str">
         <f aca="false">D43&amp;IF(B43=$E$6,"+","")</f>
@@ -6952,7 +6949,7 @@
       <c r="G43" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C43),$B$3,D43),$B$4,E43),$B$5,F43)</f>
         <v>
-BCT_Artifacts_Q7_2;2 x §MQ7§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q7_2;2 x §lQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6974,7 +6971,7 @@
       </c>
       <c r="E44" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A44,$E$2:$E$10,1))&amp;C44&amp;INDEX($G$2:$G$10,MATCH(A44,$E$2:$E$10,1))</f>
-        <v>§MQ7§!</v>
+        <v>§lQ7§!</v>
       </c>
       <c r="F44" s="20" t="str">
         <f aca="false">D44&amp;IF(B44=$E$6,"+","")</f>
@@ -6983,7 +6980,7 @@
       <c r="G44" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C44),$B$3,D44),$B$4,E44),$B$5,F44)</f>
         <v>
-BCT_Artifacts_Q7_3;3 x §MQ7§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q7_3;3 x §lQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7005,7 +7002,7 @@
       </c>
       <c r="E45" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A45,$E$2:$E$10,1))&amp;C45&amp;INDEX($G$2:$G$10,MATCH(A45,$E$2:$E$10,1))</f>
-        <v>§MQ7§!</v>
+        <v>§lQ7§!</v>
       </c>
       <c r="F45" s="20" t="str">
         <f aca="false">D45&amp;IF(B45=$E$6,"+","")</f>
@@ -7014,7 +7011,7 @@
       <c r="G45" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C45),$B$3,D45),$B$4,E45),$B$5,F45)</f>
         <v>
-BCT_Artifacts_Q7_4;4 x §MQ7§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q7_4;4 x §lQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7036,7 +7033,7 @@
       </c>
       <c r="E46" s="19" t="str">
         <f aca="false">INDEX($F$2:$F$10,MATCH(A46,$E$2:$E$10,1))&amp;C46&amp;INDEX($G$2:$G$10,MATCH(A46,$E$2:$E$10,1))</f>
-        <v>§MQ7§!</v>
+        <v>§lQ7§!</v>
       </c>
       <c r="F46" s="20" t="str">
         <f aca="false">D46&amp;IF(B46=$E$6,"+","")</f>
@@ -7045,7 +7042,7 @@
       <c r="G46" s="9" t="str">
         <f aca="false">$B$6&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($B$1,$B$2,C46),$B$3,D46),$B$4,E46),$B$5,F46)</f>
         <v>
-BCT_Artifacts_Q7_5;5+ x §MQ7§!;;;;;;;;;;;;;x</v>
+BCT_Artifacts_Q7_5;5+ x §lQ7§!;;;;;;;;;;;;;x</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>